<commit_message>
Fix - verificação compatibilidade coordenadas completa (todos os tamanhos de barco)
</commit_message>
<xml_diff>
--- a/Protótipo posicionamento barcos.xlsx
+++ b/Protótipo posicionamento barcos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro Simões\Desktop\Prog\M10\m10-3-batalha-naval\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0C85184-BA02-4262-839A-452C299F9036}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14AEE87E-9F69-42E8-9878-4BC73AB17F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{39E4F3E0-4796-4E87-B133-DFED451204FD}"/>
+    <workbookView xWindow="-21720" yWindow="660" windowWidth="21840" windowHeight="13020" xr2:uid="{39E4F3E0-4796-4E87-B133-DFED451204FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="20">
   <si>
     <t>Batalha Naval</t>
   </si>
@@ -93,13 +93,16 @@
   </si>
   <si>
     <t>2 células</t>
+  </si>
+  <si>
+    <t>Onde podem estar as casas iniciais</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -136,8 +139,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -162,6 +172,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF9B861"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -310,35 +326,41 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -349,6 +371,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFF9B861"/>
       <color rgb="FFFF4F4F"/>
     </mruColors>
   </colors>
@@ -682,777 +705,786 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BD5BCED-8683-4ED2-A9F1-A29F4D4342D6}">
   <dimension ref="E2:AQ30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="AT26" sqref="AT26"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AL17" sqref="AL17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6" defaultRowHeight="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="5:43" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="W2" s="1" t="s">
+      <c r="W2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="1"/>
-      <c r="Z2" s="1"/>
-      <c r="AA2" s="1"/>
-      <c r="AB2" s="1"/>
-      <c r="AC2" s="1"/>
-      <c r="AD2" s="1"/>
-      <c r="AE2" s="1"/>
-      <c r="AF2" s="1"/>
+      <c r="X2" s="15"/>
+      <c r="Y2" s="15"/>
+      <c r="Z2" s="15"/>
+      <c r="AA2" s="15"/>
+      <c r="AB2" s="15"/>
+      <c r="AC2" s="15"/>
+      <c r="AD2" s="15"/>
+      <c r="AE2" s="15"/>
+      <c r="AF2" s="15"/>
+    </row>
+    <row r="3" spans="5:43" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z3" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA3" s="23"/>
+      <c r="AB3" s="23"/>
+      <c r="AC3" s="23"/>
     </row>
     <row r="4" spans="5:43" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L4" s="15">
+      <c r="L4" s="1">
         <v>0</v>
       </c>
-      <c r="M4" s="15">
+      <c r="M4" s="1">
         <v>1</v>
       </c>
-      <c r="N4" s="15">
+      <c r="N4" s="1">
         <v>2</v>
       </c>
-      <c r="O4" s="15">
+      <c r="O4" s="1">
         <v>3</v>
       </c>
-      <c r="P4" s="15">
+      <c r="P4" s="1">
         <v>4</v>
       </c>
-      <c r="Q4" s="15">
+      <c r="Q4" s="1">
         <v>5</v>
       </c>
-      <c r="R4" s="15">
+      <c r="R4" s="1">
         <v>6</v>
       </c>
-      <c r="S4" s="15">
+      <c r="S4" s="1">
         <v>7</v>
       </c>
-      <c r="T4" s="15">
+      <c r="T4" s="1">
         <v>8</v>
       </c>
-      <c r="U4" s="15">
+      <c r="U4" s="1">
         <v>9</v>
       </c>
-      <c r="AH4" s="15">
+      <c r="AH4" s="1">
         <v>0</v>
       </c>
-      <c r="AI4" s="15">
+      <c r="AI4" s="1">
         <v>1</v>
       </c>
-      <c r="AJ4" s="15">
+      <c r="AJ4" s="1">
         <v>2</v>
       </c>
-      <c r="AK4" s="15">
+      <c r="AK4" s="1">
         <v>3</v>
       </c>
-      <c r="AL4" s="15">
+      <c r="AL4" s="1">
         <v>4</v>
       </c>
-      <c r="AM4" s="15">
+      <c r="AM4" s="1">
         <v>5</v>
       </c>
-      <c r="AN4" s="15">
+      <c r="AN4" s="1">
         <v>6</v>
       </c>
-      <c r="AO4" s="15">
+      <c r="AO4" s="1">
         <v>7</v>
       </c>
-      <c r="AP4" s="15">
+      <c r="AP4" s="1">
         <v>8</v>
       </c>
-      <c r="AQ4" s="15">
+      <c r="AQ4" s="1">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="5:43" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
-      <c r="K5" s="15" t="s">
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="K5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="L5" s="14"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="3"/>
-      <c r="R5" s="6"/>
-      <c r="S5" s="6"/>
-      <c r="T5" s="6"/>
-      <c r="U5" s="7"/>
-      <c r="AB5" s="19" t="s">
+      <c r="L5" s="9"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="20"/>
+      <c r="S5" s="20"/>
+      <c r="T5" s="20"/>
+      <c r="U5" s="21"/>
+      <c r="AB5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="AC5" s="19"/>
-      <c r="AD5" s="19"/>
-      <c r="AE5" s="19"/>
-      <c r="AG5" s="15" t="s">
+      <c r="AC5" s="13"/>
+      <c r="AD5" s="13"/>
+      <c r="AE5" s="13"/>
+      <c r="AG5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="AH5" s="14"/>
-      <c r="AI5" s="3"/>
-      <c r="AJ5" s="3"/>
-      <c r="AK5" s="3"/>
-      <c r="AL5" s="3"/>
-      <c r="AM5" s="3"/>
-      <c r="AN5" s="3"/>
-      <c r="AO5" s="6"/>
-      <c r="AP5" s="6"/>
-      <c r="AQ5" s="7"/>
+      <c r="AH5" s="9"/>
+      <c r="AI5" s="2"/>
+      <c r="AJ5" s="2"/>
+      <c r="AK5" s="2"/>
+      <c r="AL5" s="2"/>
+      <c r="AM5" s="2"/>
+      <c r="AN5" s="2"/>
+      <c r="AO5" s="20"/>
+      <c r="AP5" s="20"/>
+      <c r="AQ5" s="21"/>
     </row>
     <row r="6" spans="5:43" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="K6" s="15" t="s">
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="K6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L6" s="4"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="5"/>
-      <c r="Q6" s="5"/>
-      <c r="R6" s="8"/>
-      <c r="S6" s="8"/>
-      <c r="T6" s="8"/>
-      <c r="U6" s="9"/>
-      <c r="AB6" s="2" t="s">
+      <c r="L6" s="3"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="17"/>
+      <c r="S6" s="17"/>
+      <c r="T6" s="17"/>
+      <c r="U6" s="22"/>
+      <c r="AB6" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="AC6" s="2"/>
-      <c r="AD6" s="2"/>
-      <c r="AE6" s="2"/>
-      <c r="AG6" s="15" t="s">
+      <c r="AC6" s="14"/>
+      <c r="AD6" s="14"/>
+      <c r="AE6" s="14"/>
+      <c r="AG6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="AH6" s="4"/>
-      <c r="AI6" s="5"/>
-      <c r="AJ6" s="5"/>
-      <c r="AK6" s="5"/>
-      <c r="AL6" s="5"/>
-      <c r="AM6" s="5"/>
-      <c r="AN6" s="5"/>
-      <c r="AO6" s="8"/>
-      <c r="AP6" s="8"/>
-      <c r="AQ6" s="9"/>
+      <c r="AH6" s="3"/>
+      <c r="AI6" s="4"/>
+      <c r="AJ6" s="4"/>
+      <c r="AK6" s="4"/>
+      <c r="AL6" s="4"/>
+      <c r="AM6" s="4"/>
+      <c r="AN6" s="4"/>
+      <c r="AO6" s="17"/>
+      <c r="AP6" s="17"/>
+      <c r="AQ6" s="22"/>
     </row>
     <row r="7" spans="5:43" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K7" s="15" t="s">
+      <c r="K7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="L7" s="4"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
-      <c r="P7" s="5"/>
-      <c r="Q7" s="5"/>
-      <c r="R7" s="8"/>
-      <c r="S7" s="8"/>
-      <c r="T7" s="8"/>
-      <c r="U7" s="9"/>
-      <c r="AB7" s="15"/>
-      <c r="AG7" s="15" t="s">
+      <c r="L7" s="3"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="17"/>
+      <c r="S7" s="17"/>
+      <c r="T7" s="17"/>
+      <c r="U7" s="22"/>
+      <c r="AB7" s="1"/>
+      <c r="AG7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="AH7" s="4"/>
-      <c r="AI7" s="5"/>
-      <c r="AJ7" s="5"/>
-      <c r="AK7" s="5"/>
-      <c r="AL7" s="5"/>
-      <c r="AM7" s="5"/>
-      <c r="AN7" s="5"/>
-      <c r="AO7" s="8"/>
-      <c r="AP7" s="8"/>
-      <c r="AQ7" s="9"/>
+      <c r="AH7" s="3"/>
+      <c r="AI7" s="4"/>
+      <c r="AJ7" s="4"/>
+      <c r="AK7" s="4"/>
+      <c r="AL7" s="4"/>
+      <c r="AM7" s="4"/>
+      <c r="AN7" s="4"/>
+      <c r="AO7" s="17"/>
+      <c r="AP7" s="17"/>
+      <c r="AQ7" s="22"/>
     </row>
     <row r="8" spans="5:43" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K8" s="15" t="s">
+      <c r="K8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L8" s="4"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="5"/>
-      <c r="Q8" s="16"/>
-      <c r="R8" s="16"/>
-      <c r="S8" s="16"/>
-      <c r="T8" s="16"/>
-      <c r="U8" s="17"/>
-      <c r="AB8" s="15"/>
-      <c r="AG8" s="15" t="s">
+      <c r="L8" s="3"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="10"/>
+      <c r="S8" s="10"/>
+      <c r="T8" s="10"/>
+      <c r="U8" s="11"/>
+      <c r="AB8" s="1"/>
+      <c r="AG8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="AH8" s="4"/>
-      <c r="AI8" s="5"/>
-      <c r="AJ8" s="5"/>
-      <c r="AK8" s="5"/>
-      <c r="AL8" s="5"/>
-      <c r="AM8" s="5"/>
-      <c r="AN8" s="16"/>
-      <c r="AO8" s="16"/>
-      <c r="AP8" s="16"/>
-      <c r="AQ8" s="17"/>
+      <c r="AH8" s="3"/>
+      <c r="AI8" s="4"/>
+      <c r="AJ8" s="4"/>
+      <c r="AK8" s="4"/>
+      <c r="AL8" s="4"/>
+      <c r="AM8" s="4"/>
+      <c r="AN8" s="10"/>
+      <c r="AO8" s="10"/>
+      <c r="AP8" s="10"/>
+      <c r="AQ8" s="11"/>
     </row>
     <row r="9" spans="5:43" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K9" s="15" t="s">
+      <c r="K9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L9" s="4"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
-      <c r="P9" s="5"/>
-      <c r="Q9" s="5"/>
-      <c r="R9" s="8"/>
-      <c r="S9" s="8"/>
-      <c r="T9" s="8"/>
-      <c r="U9" s="9"/>
-      <c r="AB9" s="15"/>
-      <c r="AG9" s="15" t="s">
+      <c r="L9" s="3"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="17"/>
+      <c r="S9" s="17"/>
+      <c r="T9" s="17"/>
+      <c r="U9" s="22"/>
+      <c r="AB9" s="1"/>
+      <c r="AG9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="AH9" s="4"/>
-      <c r="AI9" s="5"/>
-      <c r="AJ9" s="5"/>
-      <c r="AK9" s="5"/>
-      <c r="AL9" s="5"/>
-      <c r="AM9" s="5"/>
-      <c r="AN9" s="5"/>
-      <c r="AO9" s="8"/>
-      <c r="AP9" s="8"/>
-      <c r="AQ9" s="9"/>
+      <c r="AH9" s="3"/>
+      <c r="AI9" s="4"/>
+      <c r="AJ9" s="4"/>
+      <c r="AK9" s="4"/>
+      <c r="AL9" s="4"/>
+      <c r="AM9" s="4"/>
+      <c r="AN9" s="4"/>
+      <c r="AO9" s="17"/>
+      <c r="AP9" s="17"/>
+      <c r="AQ9" s="22"/>
     </row>
     <row r="10" spans="5:43" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K10" s="15" t="s">
+      <c r="K10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L10" s="4"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
-      <c r="P10" s="16"/>
-      <c r="Q10" s="5"/>
-      <c r="R10" s="8"/>
-      <c r="S10" s="8"/>
-      <c r="T10" s="8"/>
-      <c r="U10" s="9"/>
-      <c r="AB10" s="15"/>
-      <c r="AG10" s="15" t="s">
+      <c r="L10" s="3"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="4"/>
+      <c r="R10" s="17"/>
+      <c r="S10" s="17"/>
+      <c r="T10" s="17"/>
+      <c r="U10" s="22"/>
+      <c r="AB10" s="1"/>
+      <c r="AG10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="AH10" s="4"/>
-      <c r="AI10" s="5"/>
-      <c r="AJ10" s="5"/>
-      <c r="AK10" s="5"/>
-      <c r="AL10" s="5"/>
-      <c r="AM10" s="5"/>
-      <c r="AN10" s="5"/>
-      <c r="AO10" s="8"/>
-      <c r="AP10" s="8"/>
-      <c r="AQ10" s="9"/>
+      <c r="AH10" s="3"/>
+      <c r="AI10" s="4"/>
+      <c r="AJ10" s="4"/>
+      <c r="AK10" s="4"/>
+      <c r="AL10" s="4"/>
+      <c r="AM10" s="4"/>
+      <c r="AN10" s="4"/>
+      <c r="AO10" s="17"/>
+      <c r="AP10" s="17"/>
+      <c r="AQ10" s="22"/>
     </row>
     <row r="11" spans="5:43" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K11" s="15" t="s">
+      <c r="K11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L11" s="12"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="8"/>
-      <c r="O11" s="8"/>
-      <c r="P11" s="16"/>
-      <c r="Q11" s="8"/>
-      <c r="R11" s="8"/>
-      <c r="S11" s="8"/>
-      <c r="T11" s="8"/>
-      <c r="U11" s="9"/>
-      <c r="AB11" s="15"/>
-      <c r="AG11" s="15" t="s">
+      <c r="L11" s="16"/>
+      <c r="M11" s="17"/>
+      <c r="N11" s="17"/>
+      <c r="O11" s="17"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="17"/>
+      <c r="R11" s="5"/>
+      <c r="S11" s="5"/>
+      <c r="T11" s="5"/>
+      <c r="U11" s="6"/>
+      <c r="AB11" s="1"/>
+      <c r="AG11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="AH11" s="4"/>
-      <c r="AI11" s="5"/>
-      <c r="AJ11" s="5"/>
-      <c r="AK11" s="5"/>
-      <c r="AL11" s="16"/>
-      <c r="AM11" s="5"/>
-      <c r="AN11" s="5"/>
-      <c r="AO11" s="8"/>
-      <c r="AP11" s="8"/>
-      <c r="AQ11" s="9"/>
+      <c r="AH11" s="3"/>
+      <c r="AI11" s="4"/>
+      <c r="AJ11" s="4"/>
+      <c r="AK11" s="4"/>
+      <c r="AL11" s="10"/>
+      <c r="AM11" s="4"/>
+      <c r="AN11" s="4"/>
+      <c r="AO11" s="17"/>
+      <c r="AP11" s="17"/>
+      <c r="AQ11" s="22"/>
     </row>
     <row r="12" spans="5:43" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K12" s="15" t="s">
+      <c r="K12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L12" s="12"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="8"/>
-      <c r="O12" s="8"/>
-      <c r="P12" s="16"/>
-      <c r="Q12" s="8"/>
-      <c r="R12" s="8"/>
-      <c r="S12" s="8"/>
-      <c r="T12" s="8"/>
-      <c r="U12" s="9"/>
-      <c r="AB12" s="15"/>
-      <c r="AG12" s="15" t="s">
+      <c r="L12" s="16"/>
+      <c r="M12" s="17"/>
+      <c r="N12" s="17"/>
+      <c r="O12" s="17"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="17"/>
+      <c r="R12" s="5"/>
+      <c r="S12" s="5"/>
+      <c r="T12" s="5"/>
+      <c r="U12" s="6"/>
+      <c r="AB12" s="1"/>
+      <c r="AG12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="AH12" s="12"/>
-      <c r="AI12" s="8"/>
-      <c r="AJ12" s="8"/>
-      <c r="AK12" s="8"/>
-      <c r="AL12" s="16"/>
-      <c r="AM12" s="8"/>
-      <c r="AN12" s="8"/>
-      <c r="AO12" s="8"/>
-      <c r="AP12" s="8"/>
-      <c r="AQ12" s="9"/>
+      <c r="AH12" s="16"/>
+      <c r="AI12" s="17"/>
+      <c r="AJ12" s="17"/>
+      <c r="AK12" s="17"/>
+      <c r="AL12" s="10"/>
+      <c r="AM12" s="17"/>
+      <c r="AN12" s="17"/>
+      <c r="AO12" s="5"/>
+      <c r="AP12" s="5"/>
+      <c r="AQ12" s="6"/>
     </row>
     <row r="13" spans="5:43" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K13" s="15" t="s">
+      <c r="K13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L13" s="12"/>
-      <c r="M13" s="8"/>
-      <c r="N13" s="8"/>
-      <c r="O13" s="8"/>
-      <c r="P13" s="16"/>
-      <c r="Q13" s="8"/>
-      <c r="R13" s="8"/>
-      <c r="S13" s="8"/>
-      <c r="T13" s="8"/>
-      <c r="U13" s="9"/>
-      <c r="AB13" s="15"/>
-      <c r="AG13" s="15" t="s">
+      <c r="L13" s="16"/>
+      <c r="M13" s="17"/>
+      <c r="N13" s="17"/>
+      <c r="O13" s="17"/>
+      <c r="P13" s="10"/>
+      <c r="Q13" s="17"/>
+      <c r="R13" s="5"/>
+      <c r="S13" s="5"/>
+      <c r="T13" s="5"/>
+      <c r="U13" s="6"/>
+      <c r="AB13" s="1"/>
+      <c r="AG13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="AH13" s="12"/>
-      <c r="AI13" s="8"/>
-      <c r="AJ13" s="8"/>
-      <c r="AK13" s="8"/>
-      <c r="AL13" s="16"/>
-      <c r="AM13" s="8"/>
-      <c r="AN13" s="8"/>
-      <c r="AO13" s="8"/>
-      <c r="AP13" s="8"/>
-      <c r="AQ13" s="9"/>
+      <c r="AH13" s="16"/>
+      <c r="AI13" s="17"/>
+      <c r="AJ13" s="17"/>
+      <c r="AK13" s="17"/>
+      <c r="AL13" s="10"/>
+      <c r="AM13" s="17"/>
+      <c r="AN13" s="17"/>
+      <c r="AO13" s="5"/>
+      <c r="AP13" s="5"/>
+      <c r="AQ13" s="6"/>
     </row>
     <row r="14" spans="5:43" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K14" s="15" t="s">
+      <c r="K14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L14" s="13"/>
-      <c r="M14" s="10"/>
-      <c r="N14" s="10"/>
-      <c r="O14" s="10"/>
-      <c r="P14" s="18"/>
-      <c r="Q14" s="10"/>
-      <c r="R14" s="10"/>
-      <c r="S14" s="10"/>
-      <c r="T14" s="10"/>
-      <c r="U14" s="11"/>
-      <c r="AB14" s="15"/>
-      <c r="AG14" s="15" t="s">
+      <c r="L14" s="18"/>
+      <c r="M14" s="19"/>
+      <c r="N14" s="19"/>
+      <c r="O14" s="19"/>
+      <c r="P14" s="12"/>
+      <c r="Q14" s="19"/>
+      <c r="R14" s="7"/>
+      <c r="S14" s="7"/>
+      <c r="T14" s="7"/>
+      <c r="U14" s="8"/>
+      <c r="AB14" s="1"/>
+      <c r="AG14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="AH14" s="13"/>
-      <c r="AI14" s="10"/>
-      <c r="AJ14" s="10"/>
-      <c r="AK14" s="10"/>
-      <c r="AL14" s="18"/>
-      <c r="AM14" s="10"/>
-      <c r="AN14" s="10"/>
-      <c r="AO14" s="10"/>
-      <c r="AP14" s="10"/>
-      <c r="AQ14" s="11"/>
+      <c r="AH14" s="18"/>
+      <c r="AI14" s="19"/>
+      <c r="AJ14" s="19"/>
+      <c r="AK14" s="19"/>
+      <c r="AL14" s="12"/>
+      <c r="AM14" s="19"/>
+      <c r="AN14" s="19"/>
+      <c r="AO14" s="7"/>
+      <c r="AP14" s="7"/>
+      <c r="AQ14" s="8"/>
     </row>
     <row r="20" spans="5:43" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E20" s="19" t="s">
+      <c r="E20" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
-      <c r="L20" s="15">
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="L20" s="1">
         <v>0</v>
       </c>
-      <c r="M20" s="15">
+      <c r="M20" s="1">
         <v>1</v>
       </c>
-      <c r="N20" s="15">
+      <c r="N20" s="1">
         <v>2</v>
       </c>
-      <c r="O20" s="15">
+      <c r="O20" s="1">
         <v>3</v>
       </c>
-      <c r="P20" s="15">
+      <c r="P20" s="1">
         <v>4</v>
       </c>
-      <c r="Q20" s="15">
+      <c r="Q20" s="1">
         <v>5</v>
       </c>
-      <c r="R20" s="15">
+      <c r="R20" s="1">
         <v>6</v>
       </c>
-      <c r="S20" s="15">
+      <c r="S20" s="1">
         <v>7</v>
       </c>
-      <c r="T20" s="15">
+      <c r="T20" s="1">
         <v>8</v>
       </c>
-      <c r="U20" s="15">
+      <c r="U20" s="1">
         <v>9</v>
       </c>
-      <c r="AB20" s="19" t="s">
+      <c r="AB20" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="AC20" s="19"/>
-      <c r="AD20" s="19"/>
-      <c r="AE20" s="19"/>
-      <c r="AH20" s="15">
+      <c r="AC20" s="13"/>
+      <c r="AD20" s="13"/>
+      <c r="AE20" s="13"/>
+      <c r="AH20" s="1">
         <v>0</v>
       </c>
-      <c r="AI20" s="15">
+      <c r="AI20" s="1">
         <v>1</v>
       </c>
-      <c r="AJ20" s="15">
+      <c r="AJ20" s="1">
         <v>2</v>
       </c>
-      <c r="AK20" s="15">
+      <c r="AK20" s="1">
         <v>3</v>
       </c>
-      <c r="AL20" s="15">
+      <c r="AL20" s="1">
         <v>4</v>
       </c>
-      <c r="AM20" s="15">
+      <c r="AM20" s="1">
         <v>5</v>
       </c>
-      <c r="AN20" s="15">
+      <c r="AN20" s="1">
         <v>6</v>
       </c>
-      <c r="AO20" s="15">
+      <c r="AO20" s="1">
         <v>7</v>
       </c>
-      <c r="AP20" s="15">
+      <c r="AP20" s="1">
         <v>8</v>
       </c>
-      <c r="AQ20" s="15">
+      <c r="AQ20" s="1">
         <v>9</v>
       </c>
     </row>
     <row r="21" spans="5:43" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E21" s="2" t="s">
+      <c r="E21" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="K21" s="15" t="s">
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="K21" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="L21" s="14"/>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
-      <c r="O21" s="3"/>
-      <c r="P21" s="3"/>
-      <c r="Q21" s="3"/>
-      <c r="R21" s="3"/>
-      <c r="S21" s="3"/>
-      <c r="T21" s="6"/>
-      <c r="U21" s="7"/>
-      <c r="AB21" s="2" t="s">
+      <c r="L21" s="9"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2"/>
+      <c r="R21" s="2"/>
+      <c r="S21" s="2"/>
+      <c r="T21" s="20"/>
+      <c r="U21" s="21"/>
+      <c r="AB21" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="AC21" s="2"/>
-      <c r="AD21" s="2"/>
-      <c r="AE21" s="2"/>
-      <c r="AG21" s="15" t="s">
+      <c r="AC21" s="14"/>
+      <c r="AD21" s="14"/>
+      <c r="AE21" s="14"/>
+      <c r="AG21" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="AH21" s="14"/>
-      <c r="AI21" s="3"/>
-      <c r="AJ21" s="3"/>
-      <c r="AK21" s="3"/>
-      <c r="AL21" s="3"/>
-      <c r="AM21" s="3"/>
-      <c r="AN21" s="3"/>
-      <c r="AO21" s="3"/>
-      <c r="AP21" s="3"/>
-      <c r="AQ21" s="7"/>
+      <c r="AH21" s="9"/>
+      <c r="AI21" s="2"/>
+      <c r="AJ21" s="2"/>
+      <c r="AK21" s="2"/>
+      <c r="AL21" s="2"/>
+      <c r="AM21" s="2"/>
+      <c r="AN21" s="2"/>
+      <c r="AO21" s="2"/>
+      <c r="AP21" s="2"/>
+      <c r="AQ21" s="21"/>
     </row>
     <row r="22" spans="5:43" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K22" s="15" t="s">
+      <c r="K22" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L22" s="4"/>
-      <c r="M22" s="5"/>
-      <c r="N22" s="5"/>
-      <c r="O22" s="5"/>
-      <c r="P22" s="5"/>
-      <c r="Q22" s="5"/>
-      <c r="R22" s="5"/>
-      <c r="S22" s="5"/>
-      <c r="T22" s="8"/>
-      <c r="U22" s="9"/>
-      <c r="AG22" s="15" t="s">
+      <c r="L22" s="3"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="4"/>
+      <c r="P22" s="4"/>
+      <c r="Q22" s="4"/>
+      <c r="R22" s="4"/>
+      <c r="S22" s="4"/>
+      <c r="T22" s="17"/>
+      <c r="U22" s="22"/>
+      <c r="AG22" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="AH22" s="4"/>
-      <c r="AI22" s="5"/>
-      <c r="AJ22" s="5"/>
-      <c r="AK22" s="5"/>
-      <c r="AL22" s="5"/>
-      <c r="AM22" s="5"/>
-      <c r="AN22" s="5"/>
-      <c r="AO22" s="5"/>
-      <c r="AP22" s="5"/>
-      <c r="AQ22" s="9"/>
+      <c r="AH22" s="3"/>
+      <c r="AI22" s="4"/>
+      <c r="AJ22" s="4"/>
+      <c r="AK22" s="4"/>
+      <c r="AL22" s="4"/>
+      <c r="AM22" s="4"/>
+      <c r="AN22" s="4"/>
+      <c r="AO22" s="4"/>
+      <c r="AP22" s="4"/>
+      <c r="AQ22" s="22"/>
     </row>
     <row r="23" spans="5:43" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K23" s="15" t="s">
+      <c r="K23" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="L23" s="4"/>
-      <c r="M23" s="5"/>
-      <c r="N23" s="5"/>
-      <c r="O23" s="5"/>
-      <c r="P23" s="5"/>
-      <c r="Q23" s="5"/>
-      <c r="R23" s="5"/>
-      <c r="S23" s="5"/>
-      <c r="T23" s="8"/>
-      <c r="U23" s="9"/>
-      <c r="AG23" s="15" t="s">
+      <c r="L23" s="3"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="4"/>
+      <c r="O23" s="4"/>
+      <c r="P23" s="4"/>
+      <c r="Q23" s="4"/>
+      <c r="R23" s="4"/>
+      <c r="S23" s="4"/>
+      <c r="T23" s="17"/>
+      <c r="U23" s="22"/>
+      <c r="AG23" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="AH23" s="4"/>
-      <c r="AI23" s="5"/>
-      <c r="AJ23" s="5"/>
-      <c r="AK23" s="5"/>
-      <c r="AL23" s="5"/>
-      <c r="AM23" s="5"/>
-      <c r="AN23" s="5"/>
-      <c r="AO23" s="5"/>
-      <c r="AP23" s="5"/>
-      <c r="AQ23" s="9"/>
+      <c r="AH23" s="3"/>
+      <c r="AI23" s="4"/>
+      <c r="AJ23" s="4"/>
+      <c r="AK23" s="4"/>
+      <c r="AL23" s="4"/>
+      <c r="AM23" s="4"/>
+      <c r="AN23" s="4"/>
+      <c r="AO23" s="4"/>
+      <c r="AP23" s="4"/>
+      <c r="AQ23" s="22"/>
     </row>
     <row r="24" spans="5:43" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K24" s="15" t="s">
+      <c r="K24" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L24" s="4"/>
-      <c r="M24" s="5"/>
-      <c r="N24" s="5"/>
-      <c r="O24" s="5"/>
-      <c r="P24" s="5"/>
-      <c r="Q24" s="5"/>
-      <c r="R24" s="5"/>
-      <c r="S24" s="16"/>
-      <c r="T24" s="16"/>
-      <c r="U24" s="17"/>
-      <c r="AG24" s="15" t="s">
+      <c r="L24" s="3"/>
+      <c r="M24" s="4"/>
+      <c r="N24" s="4"/>
+      <c r="O24" s="4"/>
+      <c r="P24" s="4"/>
+      <c r="Q24" s="4"/>
+      <c r="R24" s="4"/>
+      <c r="S24" s="10"/>
+      <c r="T24" s="10"/>
+      <c r="U24" s="11"/>
+      <c r="AG24" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="AH24" s="4"/>
-      <c r="AI24" s="5"/>
-      <c r="AJ24" s="5"/>
-      <c r="AK24" s="5"/>
-      <c r="AL24" s="5"/>
-      <c r="AM24" s="5"/>
-      <c r="AN24" s="5"/>
-      <c r="AO24" s="5"/>
-      <c r="AP24" s="16"/>
-      <c r="AQ24" s="17"/>
+      <c r="AH24" s="3"/>
+      <c r="AI24" s="4"/>
+      <c r="AJ24" s="4"/>
+      <c r="AK24" s="4"/>
+      <c r="AL24" s="4"/>
+      <c r="AM24" s="4"/>
+      <c r="AN24" s="4"/>
+      <c r="AO24" s="4"/>
+      <c r="AP24" s="10"/>
+      <c r="AQ24" s="11"/>
     </row>
     <row r="25" spans="5:43" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K25" s="15" t="s">
+      <c r="K25" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L25" s="4"/>
-      <c r="M25" s="5"/>
-      <c r="N25" s="5"/>
-      <c r="O25" s="5"/>
-      <c r="P25" s="5"/>
-      <c r="Q25" s="5"/>
-      <c r="R25" s="5"/>
-      <c r="S25" s="5"/>
-      <c r="T25" s="8"/>
-      <c r="U25" s="9"/>
-      <c r="AG25" s="15" t="s">
+      <c r="L25" s="3"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="4"/>
+      <c r="O25" s="4"/>
+      <c r="P25" s="4"/>
+      <c r="Q25" s="4"/>
+      <c r="R25" s="4"/>
+      <c r="S25" s="4"/>
+      <c r="T25" s="17"/>
+      <c r="U25" s="22"/>
+      <c r="AG25" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="AH25" s="4"/>
-      <c r="AI25" s="5"/>
-      <c r="AJ25" s="5"/>
-      <c r="AK25" s="5"/>
-      <c r="AL25" s="5"/>
-      <c r="AM25" s="5"/>
-      <c r="AN25" s="5"/>
-      <c r="AO25" s="5"/>
-      <c r="AP25" s="5"/>
-      <c r="AQ25" s="9"/>
+      <c r="AH25" s="3"/>
+      <c r="AI25" s="4"/>
+      <c r="AJ25" s="4"/>
+      <c r="AK25" s="4"/>
+      <c r="AL25" s="4"/>
+      <c r="AM25" s="4"/>
+      <c r="AN25" s="4"/>
+      <c r="AO25" s="4"/>
+      <c r="AP25" s="4"/>
+      <c r="AQ25" s="22"/>
     </row>
     <row r="26" spans="5:43" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K26" s="15" t="s">
+      <c r="K26" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L26" s="4"/>
-      <c r="M26" s="5"/>
-      <c r="N26" s="5"/>
-      <c r="O26" s="5"/>
-      <c r="P26" s="5"/>
-      <c r="Q26" s="5"/>
-      <c r="R26" s="5"/>
-      <c r="S26" s="5"/>
-      <c r="T26" s="8"/>
-      <c r="U26" s="9"/>
-      <c r="AG26" s="15" t="s">
+      <c r="L26" s="3"/>
+      <c r="M26" s="4"/>
+      <c r="N26" s="4"/>
+      <c r="O26" s="4"/>
+      <c r="P26" s="4"/>
+      <c r="Q26" s="4"/>
+      <c r="R26" s="4"/>
+      <c r="S26" s="4"/>
+      <c r="T26" s="17"/>
+      <c r="U26" s="22"/>
+      <c r="AG26" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="AH26" s="4"/>
-      <c r="AI26" s="5"/>
-      <c r="AJ26" s="5"/>
-      <c r="AK26" s="5"/>
-      <c r="AL26" s="5"/>
-      <c r="AM26" s="5"/>
-      <c r="AN26" s="5"/>
-      <c r="AO26" s="5"/>
-      <c r="AP26" s="5"/>
-      <c r="AQ26" s="9"/>
+      <c r="AH26" s="3"/>
+      <c r="AI26" s="4"/>
+      <c r="AJ26" s="4"/>
+      <c r="AK26" s="4"/>
+      <c r="AL26" s="4"/>
+      <c r="AM26" s="4"/>
+      <c r="AN26" s="4"/>
+      <c r="AO26" s="4"/>
+      <c r="AP26" s="4"/>
+      <c r="AQ26" s="22"/>
     </row>
     <row r="27" spans="5:43" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K27" s="15" t="s">
+      <c r="K27" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L27" s="4"/>
-      <c r="M27" s="5"/>
-      <c r="N27" s="5"/>
-      <c r="O27" s="5"/>
-      <c r="P27" s="5"/>
-      <c r="Q27" s="5"/>
-      <c r="R27" s="5"/>
-      <c r="S27" s="5"/>
-      <c r="T27" s="8"/>
-      <c r="U27" s="9"/>
-      <c r="AG27" s="15" t="s">
+      <c r="L27" s="3"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="4"/>
+      <c r="O27" s="4"/>
+      <c r="P27" s="4"/>
+      <c r="Q27" s="4"/>
+      <c r="R27" s="4"/>
+      <c r="S27" s="4"/>
+      <c r="T27" s="17"/>
+      <c r="U27" s="22"/>
+      <c r="AG27" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="AH27" s="4"/>
-      <c r="AI27" s="5"/>
-      <c r="AJ27" s="5"/>
-      <c r="AK27" s="5"/>
-      <c r="AL27" s="5"/>
-      <c r="AM27" s="5"/>
-      <c r="AN27" s="5"/>
-      <c r="AO27" s="5"/>
-      <c r="AP27" s="5"/>
-      <c r="AQ27" s="9"/>
+      <c r="AH27" s="3"/>
+      <c r="AI27" s="4"/>
+      <c r="AJ27" s="4"/>
+      <c r="AK27" s="4"/>
+      <c r="AL27" s="4"/>
+      <c r="AM27" s="4"/>
+      <c r="AN27" s="4"/>
+      <c r="AO27" s="4"/>
+      <c r="AP27" s="4"/>
+      <c r="AQ27" s="22"/>
     </row>
     <row r="28" spans="5:43" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K28" s="15" t="s">
+      <c r="K28" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L28" s="4"/>
-      <c r="M28" s="5"/>
-      <c r="N28" s="5"/>
-      <c r="O28" s="5"/>
-      <c r="P28" s="16"/>
-      <c r="Q28" s="5"/>
-      <c r="R28" s="5"/>
-      <c r="S28" s="5"/>
-      <c r="T28" s="8"/>
-      <c r="U28" s="9"/>
-      <c r="AG28" s="15" t="s">
+      <c r="L28" s="3"/>
+      <c r="M28" s="4"/>
+      <c r="N28" s="4"/>
+      <c r="O28" s="4"/>
+      <c r="P28" s="10"/>
+      <c r="Q28" s="4"/>
+      <c r="R28" s="4"/>
+      <c r="S28" s="4"/>
+      <c r="T28" s="17"/>
+      <c r="U28" s="22"/>
+      <c r="AG28" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="AH28" s="4"/>
-      <c r="AI28" s="5"/>
-      <c r="AJ28" s="5"/>
-      <c r="AK28" s="5"/>
-      <c r="AL28" s="5"/>
-      <c r="AM28" s="5"/>
-      <c r="AN28" s="5"/>
-      <c r="AO28" s="5"/>
-      <c r="AP28" s="5"/>
-      <c r="AQ28" s="9"/>
+      <c r="AH28" s="3"/>
+      <c r="AI28" s="4"/>
+      <c r="AJ28" s="4"/>
+      <c r="AK28" s="4"/>
+      <c r="AL28" s="4"/>
+      <c r="AM28" s="4"/>
+      <c r="AN28" s="4"/>
+      <c r="AO28" s="4"/>
+      <c r="AP28" s="4"/>
+      <c r="AQ28" s="22"/>
     </row>
     <row r="29" spans="5:43" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K29" s="15" t="s">
+      <c r="K29" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L29" s="12"/>
-      <c r="M29" s="8"/>
-      <c r="N29" s="8"/>
-      <c r="O29" s="8"/>
-      <c r="P29" s="16"/>
-      <c r="Q29" s="8"/>
-      <c r="R29" s="8"/>
-      <c r="S29" s="8"/>
-      <c r="T29" s="8"/>
-      <c r="U29" s="9"/>
-      <c r="AG29" s="15" t="s">
+      <c r="L29" s="16"/>
+      <c r="M29" s="17"/>
+      <c r="N29" s="17"/>
+      <c r="O29" s="17"/>
+      <c r="P29" s="10"/>
+      <c r="Q29" s="17"/>
+      <c r="R29" s="17"/>
+      <c r="S29" s="17"/>
+      <c r="T29" s="5"/>
+      <c r="U29" s="6"/>
+      <c r="AG29" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="AH29" s="4"/>
-      <c r="AI29" s="5"/>
-      <c r="AJ29" s="5"/>
-      <c r="AK29" s="5"/>
-      <c r="AL29" s="16"/>
-      <c r="AM29" s="5"/>
-      <c r="AN29" s="5"/>
-      <c r="AO29" s="5"/>
-      <c r="AP29" s="5"/>
-      <c r="AQ29" s="9"/>
+      <c r="AH29" s="3"/>
+      <c r="AI29" s="4"/>
+      <c r="AJ29" s="4"/>
+      <c r="AK29" s="4"/>
+      <c r="AL29" s="10"/>
+      <c r="AM29" s="4"/>
+      <c r="AN29" s="4"/>
+      <c r="AO29" s="4"/>
+      <c r="AP29" s="4"/>
+      <c r="AQ29" s="22"/>
     </row>
     <row r="30" spans="5:43" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K30" s="15" t="s">
+      <c r="K30" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L30" s="13"/>
-      <c r="M30" s="10"/>
-      <c r="N30" s="10"/>
-      <c r="O30" s="10"/>
-      <c r="P30" s="18"/>
-      <c r="Q30" s="10"/>
-      <c r="R30" s="10"/>
-      <c r="S30" s="10"/>
-      <c r="T30" s="10"/>
-      <c r="U30" s="11"/>
-      <c r="AG30" s="15" t="s">
+      <c r="L30" s="18"/>
+      <c r="M30" s="19"/>
+      <c r="N30" s="19"/>
+      <c r="O30" s="19"/>
+      <c r="P30" s="12"/>
+      <c r="Q30" s="19"/>
+      <c r="R30" s="19"/>
+      <c r="S30" s="19"/>
+      <c r="T30" s="7"/>
+      <c r="U30" s="8"/>
+      <c r="AG30" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="AH30" s="13"/>
-      <c r="AI30" s="10"/>
-      <c r="AJ30" s="10"/>
-      <c r="AK30" s="10"/>
-      <c r="AL30" s="18"/>
-      <c r="AM30" s="10"/>
-      <c r="AN30" s="10"/>
-      <c r="AO30" s="10"/>
-      <c r="AP30" s="10"/>
-      <c r="AQ30" s="11"/>
+      <c r="AH30" s="18"/>
+      <c r="AI30" s="19"/>
+      <c r="AJ30" s="19"/>
+      <c r="AK30" s="19"/>
+      <c r="AL30" s="12"/>
+      <c r="AM30" s="19"/>
+      <c r="AN30" s="19"/>
+      <c r="AO30" s="19"/>
+      <c r="AP30" s="19"/>
+      <c r="AQ30" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
+    <mergeCell ref="W2:AF2"/>
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="Z3:AC3"/>
     <mergeCell ref="AB5:AE5"/>
     <mergeCell ref="AB6:AE6"/>
     <mergeCell ref="E20:H20"/>
     <mergeCell ref="E21:H21"/>
     <mergeCell ref="AB20:AE20"/>
     <mergeCell ref="AB21:AE21"/>
-    <mergeCell ref="W2:AF2"/>
-    <mergeCell ref="E5:H5"/>
-    <mergeCell ref="E6:H6"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>